<commit_message>
updating login page object
</commit_message>
<xml_diff>
--- a/suitesNames/suiteNames.xlsx
+++ b/suitesNames/suiteNames.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="912" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="320">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -989,6 +989,21 @@
   </si>
   <si>
     <t>/target/find_orchards_apihzqHrMyddQdPlHOI.html</t>
+  </si>
+  <si>
+    <t>/target/capital_bank_ui_smokeCnVpPnjAEhHSZUYP.html</t>
+  </si>
+  <si>
+    <t>/target/capital_bank_ui_smokewQkoayDSNehaUcJx.html</t>
+  </si>
+  <si>
+    <t>/target/capital_bank_ui_smokeKHaoDVQdroGjXngu.html</t>
+  </si>
+  <si>
+    <t>/target/capital_bank_ui_smokeQHTkfftiDnLtmkFW.html</t>
+  </si>
+  <si>
+    <t>/target/capital_bank_ui_smokeLfPBgUEGiAPfgYWC.html</t>
   </si>
 </sst>
 </file>
@@ -2609,7 +2624,7 @@
         <v>16</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>20</v>
+        <v>319</v>
       </c>
       <c r="C2" s="27" t="s">
         <v>19</v>
@@ -2626,7 +2641,7 @@
         <v>18</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>314</v>
+        <v>20</v>
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="30"/>

</xml_diff>